<commit_message>
add more phone numbers and update call script to use excel
</commit_message>
<xml_diff>
--- a/data/sw_phone_numbers.xlsx
+++ b/data/sw_phone_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MilesChild/Desktop/Student Value Fund/swbi/swbi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8409E0CA-B38A-7F49-AA50-7BEF0E0280E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F1516B-E0DE-5340-B3D3-670331F5AC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{BC9CF5AC-046E-7445-926E-5988A68C321E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{BC9CF5AC-046E-7445-926E-5988A68C321E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="173">
   <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>(307) 635-4500</t>
   </si>
   <si>
@@ -555,6 +549,12 @@
   </si>
   <si>
     <t>Thornton, CO 80260</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -968,7 +968,7 @@
   <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,789 +978,789 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>